<commit_message>
Asignacion de reportes a construir
</commit_message>
<xml_diff>
--- a/documentos/Propuesta y Actividades/Funcionalidad Actual A migrar Aldebaran.xlsx
+++ b/documentos/Propuesta y Actividades/Funcionalidad Actual A migrar Aldebaran.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\Promos\Repos\AldebaranWeb\AldebaranWeb\documentos\Propuesta y Actividades\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\Promos\Repos\AldebaranWeb\documentos\Propuesta y Actividades\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="795" windowWidth="29040" windowHeight="15840" tabRatio="881" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="1710" windowWidth="29040" windowHeight="15840" tabRatio="881" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tareas Generales" sheetId="27" r:id="rId1"/>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="330">
   <si>
     <t>Descripción</t>
   </si>
@@ -1695,6 +1695,12 @@
   </si>
   <si>
     <t>Estimación Nuevo Alcance</t>
+  </si>
+  <si>
+    <t>javi</t>
+  </si>
+  <si>
+    <t>ADC</t>
   </si>
 </sst>
 </file>
@@ -2137,7 +2143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2362,58 +2368,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2441,23 +2399,74 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2496,7 +2505,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{07940082-40DF-9DCA-5DDE-8E407136E01D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07940082-40DF-9DCA-5DDE-8E407136E01D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2545,7 +2554,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E9174044-E2E1-F073-2CB7-9413F79DE33E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9174044-E2E1-F073-2CB7-9413F79DE33E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2594,7 +2603,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F939A49F-4F78-05EB-A370-74E036F41DAD}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F939A49F-4F78-05EB-A370-74E036F41DAD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2643,7 +2652,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B2E4EDA9-9017-D038-5B0F-C970BA356371}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2E4EDA9-9017-D038-5B0F-C970BA356371}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2692,7 +2701,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A51B6109-4C90-4C9F-AB17-842E9B03C526}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A51B6109-4C90-4C9F-AB17-842E9B03C526}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2741,7 +2750,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4F92C183-A052-E028-A879-75BB27C0E78E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F92C183-A052-E028-A879-75BB27C0E78E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2790,7 +2799,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E4289BCA-F2B2-398A-E866-37E3C9CCF26D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4289BCA-F2B2-398A-E866-37E3C9CCF26D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2839,7 +2848,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{443EB00E-E542-5956-3CD9-C3A35B396707}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{443EB00E-E542-5956-3CD9-C3A35B396707}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2888,7 +2897,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7052C74C-6686-998B-FD45-5524ADEC184D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7052C74C-6686-998B-FD45-5524ADEC184D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2937,7 +2946,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FA373E08-B2A7-E90B-CFF3-1F0F2DECDA37}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA373E08-B2A7-E90B-CFF3-1F0F2DECDA37}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2986,7 +2995,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8DDF3154-3EF6-4F98-635E-D52F9030085A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DDF3154-3EF6-4F98-635E-D52F9030085A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3035,7 +3044,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{78C970A4-48F6-EE34-E944-13CD77CA80DC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78C970A4-48F6-EE34-E944-13CD77CA80DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3084,7 +3093,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AD6D6CF2-948F-E4B8-1271-024169463E8F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD6D6CF2-948F-E4B8-1271-024169463E8F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3133,7 +3142,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{475A8FF0-745A-0920-16E3-CEB288F689A0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{475A8FF0-745A-0920-16E3-CEB288F689A0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3182,7 +3191,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7F09EFC0-4CCB-9DC5-3663-DBFAB7C73958}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F09EFC0-4CCB-9DC5-3663-DBFAB7C73958}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3226,7 +3235,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E152AC5E-1617-61CB-50E0-FFBBCB9FB201}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E152AC5E-1617-61CB-50E0-FFBBCB9FB201}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3275,7 +3284,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D02C09C5-7B54-224B-D92D-7740C9681A39}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D02C09C5-7B54-224B-D92D-7740C9681A39}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3324,7 +3333,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7815EFCB-F4AC-1585-73BC-D3DF1AEAFEE4}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7815EFCB-F4AC-1585-73BC-D3DF1AEAFEE4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3373,7 +3382,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{248A563C-384D-DDBB-E463-F49FB9578C62}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{248A563C-384D-DDBB-E463-F49FB9578C62}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3422,7 +3431,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5751E2D3-3685-D06E-FE4C-0B8A9B477266}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5751E2D3-3685-D06E-FE4C-0B8A9B477266}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3471,7 +3480,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{54C8738B-FBA7-C588-6CC4-0A8E5C0EA502}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54C8738B-FBA7-C588-6CC4-0A8E5C0EA502}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3832,20 +3841,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="82"/>
-      <c r="B1" s="83"/>
-      <c r="C1" s="84" t="s">
+      <c r="A1" s="94"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="96" t="s">
         <v>320</v>
       </c>
-      <c r="D1" s="85"/>
+      <c r="D1" s="97"/>
       <c r="E1" s="70">
         <f>SUM(E2:E7)</f>
         <v>57</v>
       </c>
-      <c r="F1" s="84" t="s">
+      <c r="F1" s="96" t="s">
         <v>327</v>
       </c>
-      <c r="G1" s="85"/>
+      <c r="G1" s="97"/>
       <c r="H1" s="70">
         <f>SUM(H2:H7)</f>
         <v>44</v>
@@ -3877,49 +3886,49 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="97" t="s">
+    <row r="3" spans="1:8" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="106">
+      <c r="C3" s="90">
         <v>10</v>
       </c>
-      <c r="D3" s="106">
+      <c r="D3" s="90">
         <v>15</v>
       </c>
-      <c r="E3" s="106">
+      <c r="E3" s="90">
         <v>15</v>
       </c>
-      <c r="F3" s="106">
+      <c r="F3" s="90">
         <v>10</v>
       </c>
-      <c r="G3" s="106">
+      <c r="G3" s="90">
         <v>10</v>
       </c>
-      <c r="H3" s="106">
+      <c r="H3" s="90">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="97" t="s">
+    <row r="4" spans="1:8" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="106">
+      <c r="C4" s="90">
         <v>10</v>
       </c>
-      <c r="D4" s="106">
+      <c r="D4" s="90">
         <v>10</v>
       </c>
-      <c r="E4" s="106">
+      <c r="E4" s="90">
         <v>10</v>
       </c>
-      <c r="F4" s="106">
+      <c r="F4" s="90">
         <v>8</v>
       </c>
-      <c r="G4" s="106">
+      <c r="G4" s="90">
         <v>8</v>
       </c>
-      <c r="H4" s="106">
+      <c r="H4" s="90">
         <v>8</v>
       </c>
     </row>
@@ -3969,26 +3978,26 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="106" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="106" t="s">
+    <row r="7" spans="1:8" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="106">
+      <c r="C7" s="90">
         <v>10</v>
       </c>
-      <c r="D7" s="106">
+      <c r="D7" s="90">
         <v>10</v>
       </c>
-      <c r="E7" s="106">
+      <c r="E7" s="90">
         <v>10</v>
       </c>
-      <c r="F7" s="106">
+      <c r="F7" s="90">
         <v>5</v>
       </c>
-      <c r="G7" s="106">
+      <c r="G7" s="90">
         <v>5</v>
       </c>
-      <c r="H7" s="106">
+      <c r="H7" s="90">
         <v>5</v>
       </c>
     </row>
@@ -4349,22 +4358,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="82"/>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="84" t="s">
+      <c r="A1" s="94"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="96" t="s">
         <v>320</v>
       </c>
-      <c r="F1" s="85"/>
+      <c r="F1" s="97"/>
       <c r="G1" s="70">
         <f>SUM(G3:G1000)</f>
         <v>53</v>
       </c>
-      <c r="H1" s="84" t="s">
+      <c r="H1" s="96" t="s">
         <v>323</v>
       </c>
-      <c r="I1" s="85"/>
+      <c r="I1" s="97"/>
       <c r="J1" s="70">
         <f>SUM(J3:J1000)</f>
         <v>23.000000000000004</v>
@@ -4419,275 +4428,275 @@
       <c r="I3" s="66"/>
       <c r="J3" s="67"/>
     </row>
-    <row r="4" spans="1:11" s="97" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="98" t="s">
+    <row r="4" spans="1:11" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="98" t="s">
+      <c r="C4" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="99" t="s">
+      <c r="D4" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="100">
-        <v>1</v>
-      </c>
-      <c r="F4" s="101">
-        <v>1</v>
-      </c>
-      <c r="G4" s="102">
-        <v>1</v>
-      </c>
-      <c r="H4" s="100">
+      <c r="E4" s="84">
+        <v>1</v>
+      </c>
+      <c r="F4" s="85">
+        <v>1</v>
+      </c>
+      <c r="G4" s="86">
+        <v>1</v>
+      </c>
+      <c r="H4" s="84">
         <v>0.3</v>
       </c>
-      <c r="I4" s="101">
+      <c r="I4" s="85">
         <v>0.3</v>
       </c>
-      <c r="J4" s="102">
+      <c r="J4" s="86">
         <v>0.3</v>
       </c>
-      <c r="K4" s="97" t="s">
+      <c r="K4" s="82" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="97" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="98" t="s">
+    <row r="5" spans="1:11" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="98" t="s">
+      <c r="C5" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="99"/>
-      <c r="E5" s="100">
-        <v>1</v>
-      </c>
-      <c r="F5" s="101">
-        <v>1</v>
-      </c>
-      <c r="G5" s="102">
-        <v>1</v>
-      </c>
-      <c r="H5" s="100">
+      <c r="D5" s="98"/>
+      <c r="E5" s="84">
+        <v>1</v>
+      </c>
+      <c r="F5" s="85">
+        <v>1</v>
+      </c>
+      <c r="G5" s="86">
+        <v>1</v>
+      </c>
+      <c r="H5" s="84">
         <v>0.3</v>
       </c>
-      <c r="I5" s="101">
+      <c r="I5" s="85">
         <v>0.3</v>
       </c>
-      <c r="J5" s="102">
+      <c r="J5" s="86">
         <v>0.3</v>
       </c>
-      <c r="K5" s="97" t="s">
+      <c r="K5" s="82" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="97" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="98" t="s">
+    <row r="6" spans="1:11" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="83" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="98" t="s">
+      <c r="C6" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="99"/>
-      <c r="E6" s="100">
-        <v>1</v>
-      </c>
-      <c r="F6" s="101">
-        <v>1</v>
-      </c>
-      <c r="G6" s="102">
-        <v>1</v>
-      </c>
-      <c r="H6" s="100">
+      <c r="D6" s="98"/>
+      <c r="E6" s="84">
+        <v>1</v>
+      </c>
+      <c r="F6" s="85">
+        <v>1</v>
+      </c>
+      <c r="G6" s="86">
+        <v>1</v>
+      </c>
+      <c r="H6" s="84">
         <v>0.4</v>
       </c>
-      <c r="I6" s="101">
+      <c r="I6" s="85">
         <v>0.4</v>
       </c>
-      <c r="J6" s="102">
+      <c r="J6" s="86">
         <v>0.4</v>
       </c>
-      <c r="K6" s="97" t="s">
+      <c r="K6" s="82" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="97" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="98" t="s">
+    <row r="7" spans="1:11" s="82" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="98" t="s">
+      <c r="C7" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="103"/>
-      <c r="E7" s="100">
-        <v>1</v>
-      </c>
-      <c r="F7" s="101">
-        <v>1</v>
-      </c>
-      <c r="G7" s="102">
-        <v>1</v>
-      </c>
-      <c r="H7" s="100">
+      <c r="D7" s="87"/>
+      <c r="E7" s="84">
+        <v>1</v>
+      </c>
+      <c r="F7" s="85">
+        <v>1</v>
+      </c>
+      <c r="G7" s="86">
+        <v>1</v>
+      </c>
+      <c r="H7" s="84">
         <v>0.3</v>
       </c>
-      <c r="I7" s="101">
+      <c r="I7" s="85">
         <v>0.3</v>
       </c>
-      <c r="J7" s="102">
+      <c r="J7" s="86">
         <v>0.3</v>
       </c>
-      <c r="K7" s="97" t="s">
+      <c r="K7" s="82" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="97" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="98" t="s">
+    <row r="8" spans="1:11" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="83" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="98" t="s">
+      <c r="C8" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="103"/>
-      <c r="E8" s="100">
-        <v>1</v>
-      </c>
-      <c r="F8" s="101">
-        <v>1</v>
-      </c>
-      <c r="G8" s="102">
-        <v>1</v>
-      </c>
-      <c r="H8" s="100">
-        <v>1</v>
-      </c>
-      <c r="I8" s="101">
-        <v>1</v>
-      </c>
-      <c r="J8" s="102">
-        <v>1</v>
-      </c>
-      <c r="K8" s="97" t="s">
+      <c r="D8" s="87"/>
+      <c r="E8" s="84">
+        <v>1</v>
+      </c>
+      <c r="F8" s="85">
+        <v>1</v>
+      </c>
+      <c r="G8" s="86">
+        <v>1</v>
+      </c>
+      <c r="H8" s="84">
+        <v>1</v>
+      </c>
+      <c r="I8" s="85">
+        <v>1</v>
+      </c>
+      <c r="J8" s="86">
+        <v>1</v>
+      </c>
+      <c r="K8" s="82" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="97" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="98" t="s">
+    <row r="9" spans="1:11" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="98" t="s">
+      <c r="C9" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="103"/>
-      <c r="E9" s="100">
-        <v>1</v>
-      </c>
-      <c r="F9" s="101">
-        <v>1</v>
-      </c>
-      <c r="G9" s="102">
-        <v>1</v>
-      </c>
-      <c r="H9" s="100">
+      <c r="D9" s="87"/>
+      <c r="E9" s="84">
+        <v>1</v>
+      </c>
+      <c r="F9" s="85">
+        <v>1</v>
+      </c>
+      <c r="G9" s="86">
+        <v>1</v>
+      </c>
+      <c r="H9" s="84">
         <v>0.3</v>
       </c>
-      <c r="I9" s="101">
+      <c r="I9" s="85">
         <v>0.3</v>
       </c>
-      <c r="J9" s="102">
+      <c r="J9" s="86">
         <v>0.3</v>
       </c>
-      <c r="K9" s="97" t="s">
+      <c r="K9" s="82" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="97" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="98" t="s">
+    <row r="10" spans="1:11" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="83" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="98" t="s">
+      <c r="C10" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="103"/>
-      <c r="E10" s="100">
-        <v>1</v>
-      </c>
-      <c r="F10" s="101">
-        <v>1</v>
-      </c>
-      <c r="G10" s="102">
-        <v>1</v>
-      </c>
-      <c r="H10" s="100">
+      <c r="D10" s="87"/>
+      <c r="E10" s="84">
+        <v>1</v>
+      </c>
+      <c r="F10" s="85">
+        <v>1</v>
+      </c>
+      <c r="G10" s="86">
+        <v>1</v>
+      </c>
+      <c r="H10" s="84">
         <v>0.3</v>
       </c>
-      <c r="I10" s="101">
+      <c r="I10" s="85">
         <v>0.3</v>
       </c>
-      <c r="J10" s="102">
+      <c r="J10" s="86">
         <v>0.3</v>
       </c>
-      <c r="K10" s="97" t="s">
+      <c r="K10" s="82" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="97" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="98" t="s">
+    <row r="11" spans="1:11" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="98" t="s">
+      <c r="C11" s="83" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="103"/>
-      <c r="E11" s="100">
-        <v>1</v>
-      </c>
-      <c r="F11" s="101">
-        <v>1</v>
-      </c>
-      <c r="G11" s="102">
-        <v>1</v>
-      </c>
-      <c r="H11" s="100">
+      <c r="D11" s="87"/>
+      <c r="E11" s="84">
+        <v>1</v>
+      </c>
+      <c r="F11" s="85">
+        <v>1</v>
+      </c>
+      <c r="G11" s="86">
+        <v>1</v>
+      </c>
+      <c r="H11" s="84">
         <v>0.3</v>
       </c>
-      <c r="I11" s="101">
+      <c r="I11" s="85">
         <v>0.3</v>
       </c>
-      <c r="J11" s="102">
+      <c r="J11" s="86">
         <v>0.3</v>
       </c>
-      <c r="K11" s="97" t="s">
+      <c r="K11" s="82" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="97" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="98" t="s">
+    <row r="12" spans="1:11" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="98" t="s">
+      <c r="C12" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="103"/>
-      <c r="E12" s="100">
-        <v>1</v>
-      </c>
-      <c r="F12" s="101">
-        <v>1</v>
-      </c>
-      <c r="G12" s="102">
-        <v>1</v>
-      </c>
-      <c r="H12" s="100">
+      <c r="D12" s="87"/>
+      <c r="E12" s="84">
+        <v>1</v>
+      </c>
+      <c r="F12" s="85">
+        <v>1</v>
+      </c>
+      <c r="G12" s="86">
+        <v>1</v>
+      </c>
+      <c r="H12" s="84">
         <v>0.3</v>
       </c>
-      <c r="I12" s="101">
+      <c r="I12" s="85">
         <v>0.3</v>
       </c>
-      <c r="J12" s="102">
+      <c r="J12" s="86">
         <v>0.3</v>
       </c>
-      <c r="K12" s="97" t="s">
+      <c r="K12" s="82" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4754,35 +4763,35 @@
       </c>
       <c r="K14" s="43"/>
     </row>
-    <row r="15" spans="1:11" s="97" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="B15" s="98" t="s">
+    <row r="15" spans="1:11" s="82" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="B15" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="98" t="s">
+      <c r="C15" s="83" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="104" t="s">
+      <c r="D15" s="88" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="100">
-        <v>1</v>
-      </c>
-      <c r="F15" s="101">
-        <v>1</v>
-      </c>
-      <c r="G15" s="102">
-        <v>1</v>
-      </c>
-      <c r="H15" s="100">
+      <c r="E15" s="84">
+        <v>1</v>
+      </c>
+      <c r="F15" s="85">
+        <v>1</v>
+      </c>
+      <c r="G15" s="86">
+        <v>1</v>
+      </c>
+      <c r="H15" s="84">
         <v>0.3</v>
       </c>
-      <c r="I15" s="101">
+      <c r="I15" s="85">
         <v>0.3</v>
       </c>
-      <c r="J15" s="102">
+      <c r="J15" s="86">
         <v>0.3</v>
       </c>
-      <c r="K15" s="97" t="s">
+      <c r="K15" s="82" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4946,33 +4955,33 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="97" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="98" t="s">
+    <row r="21" spans="1:11" s="82" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="83" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="98" t="s">
+      <c r="C21" s="83" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="103"/>
-      <c r="E21" s="100">
-        <v>1</v>
-      </c>
-      <c r="F21" s="101">
-        <v>1</v>
-      </c>
-      <c r="G21" s="102">
-        <v>1</v>
-      </c>
-      <c r="H21" s="100">
+      <c r="D21" s="87"/>
+      <c r="E21" s="84">
+        <v>1</v>
+      </c>
+      <c r="F21" s="85">
+        <v>1</v>
+      </c>
+      <c r="G21" s="86">
+        <v>1</v>
+      </c>
+      <c r="H21" s="84">
         <v>0.3</v>
       </c>
-      <c r="I21" s="101">
+      <c r="I21" s="85">
         <v>0.3</v>
       </c>
-      <c r="J21" s="102">
+      <c r="J21" s="86">
         <v>0.3</v>
       </c>
-      <c r="K21" s="97" t="s">
+      <c r="K21" s="82" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4990,93 +4999,93 @@
       <c r="I22" s="66"/>
       <c r="J22" s="67"/>
     </row>
-    <row r="23" spans="1:11" s="97" customFormat="1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="98" t="s">
+    <row r="23" spans="1:11" s="82" customFormat="1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="83" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="98" t="s">
+      <c r="C23" s="83" t="s">
         <v>65</v>
       </c>
-      <c r="D23" s="105" t="s">
+      <c r="D23" s="89" t="s">
         <v>66</v>
       </c>
-      <c r="E23" s="100">
-        <v>1</v>
-      </c>
-      <c r="F23" s="101">
-        <v>1</v>
-      </c>
-      <c r="G23" s="102">
-        <v>1</v>
-      </c>
-      <c r="H23" s="100">
+      <c r="E23" s="84">
+        <v>1</v>
+      </c>
+      <c r="F23" s="85">
+        <v>1</v>
+      </c>
+      <c r="G23" s="86">
+        <v>1</v>
+      </c>
+      <c r="H23" s="84">
         <v>0.3</v>
       </c>
-      <c r="I23" s="101">
+      <c r="I23" s="85">
         <v>0.3</v>
       </c>
-      <c r="J23" s="102">
+      <c r="J23" s="86">
         <v>0.3</v>
       </c>
-      <c r="K23" s="97" t="s">
+      <c r="K23" s="82" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="97" customFormat="1" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="98" t="s">
+    <row r="24" spans="1:11" s="82" customFormat="1" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="83" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="98" t="s">
+      <c r="C24" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="105" t="s">
+      <c r="D24" s="89" t="s">
         <v>69</v>
       </c>
-      <c r="E24" s="100">
-        <v>1</v>
-      </c>
-      <c r="F24" s="101">
-        <v>1</v>
-      </c>
-      <c r="G24" s="102">
-        <v>1</v>
-      </c>
-      <c r="H24" s="100">
-        <v>1</v>
-      </c>
-      <c r="I24" s="101">
-        <v>1</v>
-      </c>
-      <c r="J24" s="102">
-        <v>1</v>
-      </c>
-      <c r="K24" s="97" t="s">
+      <c r="E24" s="84">
+        <v>1</v>
+      </c>
+      <c r="F24" s="85">
+        <v>1</v>
+      </c>
+      <c r="G24" s="86">
+        <v>1</v>
+      </c>
+      <c r="H24" s="84">
+        <v>1</v>
+      </c>
+      <c r="I24" s="85">
+        <v>1</v>
+      </c>
+      <c r="J24" s="86">
+        <v>1</v>
+      </c>
+      <c r="K24" s="82" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="97" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="98" t="s">
+    <row r="25" spans="1:11" s="82" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="83" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="98" t="s">
+      <c r="C25" s="83" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="105" t="s">
+      <c r="D25" s="89" t="s">
         <v>72</v>
       </c>
-      <c r="E25" s="100"/>
-      <c r="F25" s="101"/>
-      <c r="G25" s="102"/>
-      <c r="H25" s="100">
-        <v>1</v>
-      </c>
-      <c r="I25" s="101">
-        <v>1</v>
-      </c>
-      <c r="J25" s="102">
-        <v>1</v>
-      </c>
-      <c r="K25" s="97" t="s">
+      <c r="E25" s="84"/>
+      <c r="F25" s="85"/>
+      <c r="G25" s="86"/>
+      <c r="H25" s="84">
+        <v>1</v>
+      </c>
+      <c r="I25" s="85">
+        <v>1</v>
+      </c>
+      <c r="J25" s="86">
+        <v>1</v>
+      </c>
+      <c r="K25" s="82" t="s">
         <v>57</v>
       </c>
     </row>
@@ -5111,7 +5120,7 @@
       </c>
       <c r="K26" s="37"/>
     </row>
-    <row r="27" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="43"/>
       <c r="B27" s="44" t="s">
         <v>67</v>
@@ -5122,13 +5131,13 @@
       <c r="D27" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="E27" s="87">
+      <c r="E27" s="100">
         <v>4</v>
       </c>
-      <c r="F27" s="87">
+      <c r="F27" s="100">
         <v>3</v>
       </c>
-      <c r="G27" s="87">
+      <c r="G27" s="100">
         <v>3</v>
       </c>
       <c r="H27" s="19">
@@ -5153,9 +5162,9 @@
       <c r="D28" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="E28" s="87"/>
-      <c r="F28" s="87"/>
-      <c r="G28" s="87"/>
+      <c r="E28" s="100"/>
+      <c r="F28" s="100"/>
+      <c r="G28" s="100"/>
       <c r="H28" s="19">
         <v>0</v>
       </c>
@@ -5264,63 +5273,63 @@
       <c r="I32" s="66"/>
       <c r="J32" s="67"/>
     </row>
-    <row r="33" spans="1:11" s="97" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B33" s="98" t="s">
+    <row r="33" spans="1:11" s="82" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B33" s="83" t="s">
         <v>90</v>
       </c>
-      <c r="C33" s="98" t="s">
+      <c r="C33" s="83" t="s">
         <v>91</v>
       </c>
-      <c r="D33" s="103"/>
-      <c r="E33" s="100">
-        <v>1</v>
-      </c>
-      <c r="F33" s="101">
-        <v>1</v>
-      </c>
-      <c r="G33" s="102">
-        <v>1</v>
-      </c>
-      <c r="H33" s="100">
+      <c r="D33" s="87"/>
+      <c r="E33" s="84">
+        <v>1</v>
+      </c>
+      <c r="F33" s="85">
+        <v>1</v>
+      </c>
+      <c r="G33" s="86">
+        <v>1</v>
+      </c>
+      <c r="H33" s="84">
         <v>0.3</v>
       </c>
-      <c r="I33" s="101">
+      <c r="I33" s="85">
         <v>0.3</v>
       </c>
-      <c r="J33" s="102">
+      <c r="J33" s="86">
         <v>0.3</v>
       </c>
-      <c r="K33" s="97" t="s">
+      <c r="K33" s="82" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:11" s="97" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B34" s="98" t="s">
+    <row r="34" spans="1:11" s="82" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B34" s="83" t="s">
         <v>92</v>
       </c>
-      <c r="C34" s="98" t="s">
+      <c r="C34" s="83" t="s">
         <v>93</v>
       </c>
-      <c r="D34" s="103"/>
-      <c r="E34" s="100">
-        <v>1</v>
-      </c>
-      <c r="F34" s="101">
-        <v>1</v>
-      </c>
-      <c r="G34" s="102">
-        <v>1</v>
-      </c>
-      <c r="H34" s="100">
+      <c r="D34" s="87"/>
+      <c r="E34" s="84">
+        <v>1</v>
+      </c>
+      <c r="F34" s="85">
+        <v>1</v>
+      </c>
+      <c r="G34" s="86">
+        <v>1</v>
+      </c>
+      <c r="H34" s="84">
         <v>0.3</v>
       </c>
-      <c r="I34" s="101">
+      <c r="I34" s="85">
         <v>0.3</v>
       </c>
-      <c r="J34" s="102">
+      <c r="J34" s="86">
         <v>0.3</v>
       </c>
-      <c r="K34" s="97" t="s">
+      <c r="K34" s="82" t="s">
         <v>23</v>
       </c>
     </row>
@@ -5336,93 +5345,93 @@
       <c r="I35" s="66"/>
       <c r="J35" s="67"/>
     </row>
-    <row r="36" spans="1:11" s="97" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="98" t="s">
+    <row r="36" spans="1:11" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="83" t="s">
         <v>95</v>
       </c>
-      <c r="C36" s="98" t="s">
+      <c r="C36" s="83" t="s">
         <v>96</v>
       </c>
-      <c r="D36" s="103"/>
-      <c r="E36" s="100">
+      <c r="D36" s="87"/>
+      <c r="E36" s="84">
         <v>2</v>
       </c>
-      <c r="F36" s="101">
+      <c r="F36" s="85">
         <v>2</v>
       </c>
-      <c r="G36" s="102">
+      <c r="G36" s="86">
         <v>2</v>
       </c>
-      <c r="H36" s="100">
+      <c r="H36" s="84">
         <v>2</v>
       </c>
-      <c r="I36" s="101">
+      <c r="I36" s="85">
         <v>2</v>
       </c>
-      <c r="J36" s="102">
+      <c r="J36" s="86">
         <v>2</v>
       </c>
-      <c r="K36" s="97" t="s">
+      <c r="K36" s="82" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="97" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="98" t="s">
+    <row r="37" spans="1:11" s="82" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="83" t="s">
         <v>97</v>
       </c>
-      <c r="C37" s="98" t="s">
+      <c r="C37" s="83" t="s">
         <v>98</v>
       </c>
-      <c r="D37" s="103"/>
-      <c r="E37" s="100">
-        <v>1</v>
-      </c>
-      <c r="F37" s="101">
-        <v>1</v>
-      </c>
-      <c r="G37" s="102">
-        <v>1</v>
-      </c>
-      <c r="H37" s="100">
-        <v>1</v>
-      </c>
-      <c r="I37" s="101">
-        <v>1</v>
-      </c>
-      <c r="J37" s="102">
-        <v>1</v>
-      </c>
-      <c r="K37" s="97" t="s">
+      <c r="D37" s="87"/>
+      <c r="E37" s="84">
+        <v>1</v>
+      </c>
+      <c r="F37" s="85">
+        <v>1</v>
+      </c>
+      <c r="G37" s="86">
+        <v>1</v>
+      </c>
+      <c r="H37" s="84">
+        <v>1</v>
+      </c>
+      <c r="I37" s="85">
+        <v>1</v>
+      </c>
+      <c r="J37" s="86">
+        <v>1</v>
+      </c>
+      <c r="K37" s="82" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="1:11" s="97" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="98" t="s">
+    <row r="38" spans="1:11" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="83" t="s">
         <v>99</v>
       </c>
-      <c r="C38" s="98" t="s">
+      <c r="C38" s="83" t="s">
         <v>100</v>
       </c>
-      <c r="D38" s="103"/>
-      <c r="E38" s="100">
-        <v>1</v>
-      </c>
-      <c r="F38" s="101">
-        <v>1</v>
-      </c>
-      <c r="G38" s="102">
-        <v>1</v>
-      </c>
-      <c r="H38" s="100">
-        <v>1</v>
-      </c>
-      <c r="I38" s="101">
-        <v>1</v>
-      </c>
-      <c r="J38" s="102">
-        <v>1</v>
-      </c>
-      <c r="K38" s="97" t="s">
+      <c r="D38" s="87"/>
+      <c r="E38" s="84">
+        <v>1</v>
+      </c>
+      <c r="F38" s="85">
+        <v>1</v>
+      </c>
+      <c r="G38" s="86">
+        <v>1</v>
+      </c>
+      <c r="H38" s="84">
+        <v>1</v>
+      </c>
+      <c r="I38" s="85">
+        <v>1</v>
+      </c>
+      <c r="J38" s="86">
+        <v>1</v>
+      </c>
+      <c r="K38" s="82" t="s">
         <v>57</v>
       </c>
     </row>
@@ -5463,95 +5472,95 @@
       <c r="I40" s="66"/>
       <c r="J40" s="67"/>
     </row>
-    <row r="41" spans="1:11" s="97" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B41" s="98" t="s">
+    <row r="41" spans="1:11" s="82" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B41" s="83" t="s">
         <v>103</v>
       </c>
-      <c r="C41" s="98" t="s">
+      <c r="C41" s="83" t="s">
         <v>104</v>
       </c>
-      <c r="D41" s="99" t="s">
+      <c r="D41" s="98" t="s">
         <v>105</v>
       </c>
-      <c r="E41" s="100">
-        <v>1</v>
-      </c>
-      <c r="F41" s="101">
-        <v>1</v>
-      </c>
-      <c r="G41" s="102">
-        <v>1</v>
-      </c>
-      <c r="H41" s="100">
+      <c r="E41" s="84">
+        <v>1</v>
+      </c>
+      <c r="F41" s="85">
+        <v>1</v>
+      </c>
+      <c r="G41" s="86">
+        <v>1</v>
+      </c>
+      <c r="H41" s="84">
         <v>0.3</v>
       </c>
-      <c r="I41" s="101">
+      <c r="I41" s="85">
         <v>0.3</v>
       </c>
-      <c r="J41" s="102">
+      <c r="J41" s="86">
         <v>0.3</v>
       </c>
-      <c r="K41" s="97" t="s">
+      <c r="K41" s="82" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:11" s="97" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="98" t="s">
+    <row r="42" spans="1:11" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="83" t="s">
         <v>102</v>
       </c>
-      <c r="C42" s="98" t="s">
+      <c r="C42" s="83" t="s">
         <v>106</v>
       </c>
-      <c r="D42" s="99"/>
-      <c r="E42" s="100">
-        <v>1</v>
-      </c>
-      <c r="F42" s="101">
-        <v>1</v>
-      </c>
-      <c r="G42" s="102">
-        <v>1</v>
-      </c>
-      <c r="H42" s="100">
+      <c r="D42" s="98"/>
+      <c r="E42" s="84">
+        <v>1</v>
+      </c>
+      <c r="F42" s="85">
+        <v>1</v>
+      </c>
+      <c r="G42" s="86">
+        <v>1</v>
+      </c>
+      <c r="H42" s="84">
         <v>0.3</v>
       </c>
-      <c r="I42" s="101">
+      <c r="I42" s="85">
         <v>0.3</v>
       </c>
-      <c r="J42" s="102">
+      <c r="J42" s="86">
         <v>0.3</v>
       </c>
-      <c r="K42" s="97" t="s">
+      <c r="K42" s="82" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:11" s="97" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B43" s="98" t="s">
+    <row r="43" spans="1:11" s="82" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B43" s="83" t="s">
         <v>107</v>
       </c>
-      <c r="C43" s="98" t="s">
+      <c r="C43" s="83" t="s">
         <v>108</v>
       </c>
-      <c r="D43" s="99"/>
-      <c r="E43" s="100">
-        <v>1</v>
-      </c>
-      <c r="F43" s="101">
-        <v>1</v>
-      </c>
-      <c r="G43" s="102">
-        <v>1</v>
-      </c>
-      <c r="H43" s="100">
+      <c r="D43" s="98"/>
+      <c r="E43" s="84">
+        <v>1</v>
+      </c>
+      <c r="F43" s="85">
+        <v>1</v>
+      </c>
+      <c r="G43" s="86">
+        <v>1</v>
+      </c>
+      <c r="H43" s="84">
         <v>0.3</v>
       </c>
-      <c r="I43" s="101">
+      <c r="I43" s="85">
         <v>0.3</v>
       </c>
-      <c r="J43" s="102">
+      <c r="J43" s="86">
         <v>0.3</v>
       </c>
-      <c r="K43" s="97" t="s">
+      <c r="K43" s="82" t="s">
         <v>23</v>
       </c>
     </row>
@@ -5644,153 +5653,153 @@
       </c>
       <c r="K47" s="43"/>
     </row>
-    <row r="48" spans="1:11" s="97" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="98" t="s">
+    <row r="48" spans="1:11" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="83" t="s">
         <v>116</v>
       </c>
-      <c r="C48" s="98" t="s">
+      <c r="C48" s="83" t="s">
         <v>117</v>
       </c>
-      <c r="D48" s="103"/>
-      <c r="E48" s="100">
-        <v>1</v>
-      </c>
-      <c r="F48" s="101">
-        <v>1</v>
-      </c>
-      <c r="G48" s="102">
-        <v>1</v>
-      </c>
-      <c r="H48" s="100">
-        <v>1</v>
-      </c>
-      <c r="I48" s="101">
-        <v>1</v>
-      </c>
-      <c r="J48" s="102">
-        <v>1</v>
-      </c>
-      <c r="K48" s="97" t="s">
+      <c r="D48" s="87"/>
+      <c r="E48" s="84">
+        <v>1</v>
+      </c>
+      <c r="F48" s="85">
+        <v>1</v>
+      </c>
+      <c r="G48" s="86">
+        <v>1</v>
+      </c>
+      <c r="H48" s="84">
+        <v>1</v>
+      </c>
+      <c r="I48" s="85">
+        <v>1</v>
+      </c>
+      <c r="J48" s="86">
+        <v>1</v>
+      </c>
+      <c r="K48" s="82" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="49" spans="2:11" s="97" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="98" t="s">
+    <row r="49" spans="2:11" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="83" t="s">
         <v>118</v>
       </c>
-      <c r="C49" s="98" t="s">
+      <c r="C49" s="83" t="s">
         <v>119</v>
       </c>
-      <c r="D49" s="103"/>
-      <c r="E49" s="100">
-        <v>1</v>
-      </c>
-      <c r="F49" s="101">
-        <v>1</v>
-      </c>
-      <c r="G49" s="102">
-        <v>1</v>
-      </c>
-      <c r="H49" s="100">
-        <v>1</v>
-      </c>
-      <c r="I49" s="101">
-        <v>1</v>
-      </c>
-      <c r="J49" s="102">
-        <v>1</v>
-      </c>
-      <c r="K49" s="97" t="s">
+      <c r="D49" s="87"/>
+      <c r="E49" s="84">
+        <v>1</v>
+      </c>
+      <c r="F49" s="85">
+        <v>1</v>
+      </c>
+      <c r="G49" s="86">
+        <v>1</v>
+      </c>
+      <c r="H49" s="84">
+        <v>1</v>
+      </c>
+      <c r="I49" s="85">
+        <v>1</v>
+      </c>
+      <c r="J49" s="86">
+        <v>1</v>
+      </c>
+      <c r="K49" s="82" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="50" spans="2:11" s="97" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B50" s="98" t="s">
+    <row r="50" spans="2:11" s="82" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B50" s="83" t="s">
         <v>120</v>
       </c>
-      <c r="C50" s="98" t="s">
+      <c r="C50" s="83" t="s">
         <v>121</v>
       </c>
-      <c r="D50" s="103"/>
-      <c r="E50" s="100">
-        <v>1</v>
-      </c>
-      <c r="F50" s="101">
-        <v>1</v>
-      </c>
-      <c r="G50" s="102">
-        <v>1</v>
-      </c>
-      <c r="H50" s="100">
-        <v>1</v>
-      </c>
-      <c r="I50" s="101">
-        <v>1</v>
-      </c>
-      <c r="J50" s="102">
-        <v>1</v>
-      </c>
-      <c r="K50" s="97" t="s">
+      <c r="D50" s="87"/>
+      <c r="E50" s="84">
+        <v>1</v>
+      </c>
+      <c r="F50" s="85">
+        <v>1</v>
+      </c>
+      <c r="G50" s="86">
+        <v>1</v>
+      </c>
+      <c r="H50" s="84">
+        <v>1</v>
+      </c>
+      <c r="I50" s="85">
+        <v>1</v>
+      </c>
+      <c r="J50" s="86">
+        <v>1</v>
+      </c>
+      <c r="K50" s="82" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="2:11" s="97" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B51" s="98" t="s">
+    <row r="51" spans="2:11" s="82" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B51" s="83" t="s">
         <v>122</v>
       </c>
-      <c r="C51" s="98" t="s">
+      <c r="C51" s="83" t="s">
         <v>123</v>
       </c>
-      <c r="D51" s="103"/>
-      <c r="E51" s="100">
-        <v>1</v>
-      </c>
-      <c r="F51" s="101">
-        <v>1</v>
-      </c>
-      <c r="G51" s="102">
-        <v>1</v>
-      </c>
-      <c r="H51" s="100">
-        <v>1</v>
-      </c>
-      <c r="I51" s="101">
-        <v>1</v>
-      </c>
-      <c r="J51" s="102">
-        <v>1</v>
-      </c>
-      <c r="K51" s="97" t="s">
+      <c r="D51" s="87"/>
+      <c r="E51" s="84">
+        <v>1</v>
+      </c>
+      <c r="F51" s="85">
+        <v>1</v>
+      </c>
+      <c r="G51" s="86">
+        <v>1</v>
+      </c>
+      <c r="H51" s="84">
+        <v>1</v>
+      </c>
+      <c r="I51" s="85">
+        <v>1</v>
+      </c>
+      <c r="J51" s="86">
+        <v>1</v>
+      </c>
+      <c r="K51" s="82" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="52" spans="2:11" s="97" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B52" s="98" t="s">
+    <row r="52" spans="2:11" s="82" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B52" s="83" t="s">
         <v>124</v>
       </c>
-      <c r="C52" s="98" t="s">
+      <c r="C52" s="83" t="s">
         <v>125</v>
       </c>
-      <c r="D52" s="103"/>
-      <c r="E52" s="100">
-        <v>1</v>
-      </c>
-      <c r="F52" s="101">
-        <v>1</v>
-      </c>
-      <c r="G52" s="102">
-        <v>1</v>
-      </c>
-      <c r="H52" s="100">
-        <v>1</v>
-      </c>
-      <c r="I52" s="101">
-        <v>1</v>
-      </c>
-      <c r="J52" s="102">
-        <v>1</v>
-      </c>
-      <c r="K52" s="97" t="s">
+      <c r="D52" s="87"/>
+      <c r="E52" s="84">
+        <v>1</v>
+      </c>
+      <c r="F52" s="85">
+        <v>1</v>
+      </c>
+      <c r="G52" s="86">
+        <v>1</v>
+      </c>
+      <c r="H52" s="84">
+        <v>1</v>
+      </c>
+      <c r="I52" s="85">
+        <v>1</v>
+      </c>
+      <c r="J52" s="86">
+        <v>1</v>
+      </c>
+      <c r="K52" s="82" t="s">
         <v>57</v>
       </c>
     </row>
@@ -6355,9 +6364,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A62" sqref="A62:XFD62"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6379,22 +6388,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="91"/>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="88" t="s">
+      <c r="A1" s="105"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="109" t="s">
         <v>320</v>
       </c>
-      <c r="F1" s="89"/>
+      <c r="F1" s="110"/>
       <c r="G1" s="71">
         <f>SUM(G2:G1000)</f>
         <v>207</v>
       </c>
-      <c r="H1" s="88" t="s">
+      <c r="H1" s="109" t="s">
         <v>323</v>
       </c>
-      <c r="I1" s="89"/>
+      <c r="I1" s="110"/>
       <c r="J1" s="71">
         <f>SUM(J2:J1000)</f>
         <v>131</v>
@@ -6440,223 +6449,223 @@
       <c r="L3" s="62"/>
       <c r="M3" s="62"/>
     </row>
-    <row r="4" spans="1:13" s="98" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="107" t="s">
+    <row r="4" spans="1:13" s="83" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="104" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="107" t="s">
+      <c r="C4" s="104" t="s">
         <v>128</v>
       </c>
-      <c r="D4" s="108" t="s">
+      <c r="D4" s="102" t="s">
         <v>129</v>
       </c>
-      <c r="E4" s="109">
+      <c r="E4" s="103">
         <v>10</v>
       </c>
-      <c r="F4" s="109">
+      <c r="F4" s="103">
         <v>15</v>
       </c>
-      <c r="G4" s="109">
+      <c r="G4" s="103">
         <v>15</v>
       </c>
-      <c r="H4" s="109">
+      <c r="H4" s="103">
         <v>10</v>
       </c>
-      <c r="I4" s="109">
+      <c r="I4" s="103">
         <v>10</v>
       </c>
-      <c r="J4" s="109">
+      <c r="J4" s="103">
         <v>10</v>
       </c>
-      <c r="K4" s="109" t="s">
+      <c r="K4" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="L4" s="109"/>
-      <c r="M4" s="109"/>
-    </row>
-    <row r="5" spans="1:13" s="98" customFormat="1" ht="272.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="107"/>
-      <c r="C5" s="107"/>
-      <c r="D5" s="110"/>
-      <c r="E5" s="109"/>
-      <c r="F5" s="109"/>
-      <c r="G5" s="109"/>
-      <c r="H5" s="109"/>
-      <c r="I5" s="109"/>
-      <c r="J5" s="109"/>
-      <c r="K5" s="109"/>
-      <c r="L5" s="109"/>
-      <c r="M5" s="109"/>
-    </row>
-    <row r="6" spans="1:13" s="98" customFormat="1" ht="300" x14ac:dyDescent="0.25">
-      <c r="B6" s="98" t="s">
+      <c r="L4" s="103"/>
+      <c r="M4" s="103"/>
+    </row>
+    <row r="5" spans="1:13" s="83" customFormat="1" ht="272.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="104"/>
+      <c r="C5" s="104"/>
+      <c r="D5" s="108"/>
+      <c r="E5" s="103"/>
+      <c r="F5" s="103"/>
+      <c r="G5" s="103"/>
+      <c r="H5" s="103"/>
+      <c r="I5" s="103"/>
+      <c r="J5" s="103"/>
+      <c r="K5" s="103"/>
+      <c r="L5" s="103"/>
+      <c r="M5" s="103"/>
+    </row>
+    <row r="6" spans="1:13" s="83" customFormat="1" ht="300" x14ac:dyDescent="0.25">
+      <c r="B6" s="83" t="s">
         <v>130</v>
       </c>
-      <c r="C6" s="98" t="s">
+      <c r="C6" s="83" t="s">
         <v>131</v>
       </c>
-      <c r="D6" s="111" t="s">
+      <c r="D6" s="92" t="s">
         <v>132</v>
       </c>
-      <c r="E6" s="98">
+      <c r="E6" s="83">
         <v>7</v>
       </c>
-      <c r="F6" s="98">
+      <c r="F6" s="83">
         <v>7</v>
       </c>
-      <c r="G6" s="98">
+      <c r="G6" s="83">
         <v>7</v>
       </c>
-      <c r="H6" s="98">
+      <c r="H6" s="83">
         <v>4</v>
       </c>
-      <c r="I6" s="98">
+      <c r="I6" s="83">
         <v>4</v>
       </c>
-      <c r="J6" s="98">
+      <c r="J6" s="83">
         <v>4</v>
       </c>
-      <c r="K6" s="97" t="s">
+      <c r="K6" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="L6" s="97"/>
-      <c r="M6" s="97"/>
-    </row>
-    <row r="7" spans="1:13" s="98" customFormat="1" ht="390" x14ac:dyDescent="0.25">
-      <c r="B7" s="98" t="s">
+      <c r="L6" s="82"/>
+      <c r="M6" s="82"/>
+    </row>
+    <row r="7" spans="1:13" s="83" customFormat="1" ht="390" x14ac:dyDescent="0.25">
+      <c r="B7" s="83" t="s">
         <v>133</v>
       </c>
-      <c r="C7" s="98" t="s">
+      <c r="C7" s="83" t="s">
         <v>134</v>
       </c>
-      <c r="D7" s="111" t="s">
+      <c r="D7" s="92" t="s">
         <v>135</v>
       </c>
-      <c r="E7" s="98">
+      <c r="E7" s="83">
         <v>7</v>
       </c>
-      <c r="F7" s="98">
+      <c r="F7" s="83">
         <v>7</v>
       </c>
-      <c r="G7" s="98">
+      <c r="G7" s="83">
         <v>7</v>
       </c>
-      <c r="H7" s="98">
+      <c r="H7" s="83">
         <v>4</v>
       </c>
-      <c r="I7" s="98">
+      <c r="I7" s="83">
         <v>4</v>
       </c>
-      <c r="J7" s="98">
+      <c r="J7" s="83">
         <v>4</v>
       </c>
-      <c r="K7" s="97" t="s">
+      <c r="K7" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="L7" s="97"/>
-      <c r="M7" s="97"/>
-    </row>
-    <row r="8" spans="1:13" s="98" customFormat="1" ht="199.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="98" t="s">
+      <c r="L7" s="82"/>
+      <c r="M7" s="82"/>
+    </row>
+    <row r="8" spans="1:13" s="83" customFormat="1" ht="199.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="83" t="s">
         <v>136</v>
       </c>
-      <c r="C8" s="98" t="s">
+      <c r="C8" s="83" t="s">
         <v>137</v>
       </c>
-      <c r="D8" s="111" t="s">
+      <c r="D8" s="92" t="s">
         <v>138</v>
       </c>
-      <c r="E8" s="98">
+      <c r="E8" s="83">
         <v>5</v>
       </c>
-      <c r="F8" s="98">
+      <c r="F8" s="83">
         <v>5</v>
       </c>
-      <c r="G8" s="98">
+      <c r="G8" s="83">
         <v>5</v>
       </c>
-      <c r="H8" s="98">
+      <c r="H8" s="83">
         <v>4</v>
       </c>
-      <c r="I8" s="98">
+      <c r="I8" s="83">
         <v>4</v>
       </c>
-      <c r="J8" s="98">
+      <c r="J8" s="83">
         <v>4</v>
       </c>
-      <c r="K8" s="97" t="s">
+      <c r="K8" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="97"/>
-      <c r="M8" s="97"/>
-    </row>
-    <row r="9" spans="1:13" s="98" customFormat="1" ht="165" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="98" t="s">
+      <c r="L8" s="82"/>
+      <c r="M8" s="82"/>
+    </row>
+    <row r="9" spans="1:13" s="83" customFormat="1" ht="165" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="83" t="s">
         <v>139</v>
       </c>
-      <c r="C9" s="98" t="s">
+      <c r="C9" s="83" t="s">
         <v>140</v>
       </c>
-      <c r="D9" s="112" t="s">
+      <c r="D9" s="93" t="s">
         <v>141</v>
       </c>
-      <c r="E9" s="98">
+      <c r="E9" s="83">
         <v>2</v>
       </c>
-      <c r="F9" s="98">
+      <c r="F9" s="83">
         <v>2</v>
       </c>
-      <c r="G9" s="98">
+      <c r="G9" s="83">
         <v>2</v>
       </c>
-      <c r="H9" s="98">
+      <c r="H9" s="83">
         <v>2</v>
       </c>
-      <c r="I9" s="98">
+      <c r="I9" s="83">
         <v>2</v>
       </c>
-      <c r="J9" s="98">
+      <c r="J9" s="83">
         <v>2</v>
       </c>
-      <c r="K9" s="97" t="s">
+      <c r="K9" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="L9" s="97"/>
-      <c r="M9" s="97"/>
-    </row>
-    <row r="10" spans="1:13" s="98" customFormat="1" ht="225" x14ac:dyDescent="0.25">
-      <c r="B10" s="98" t="s">
+      <c r="L9" s="82"/>
+      <c r="M9" s="82"/>
+    </row>
+    <row r="10" spans="1:13" s="83" customFormat="1" ht="225" x14ac:dyDescent="0.25">
+      <c r="B10" s="83" t="s">
         <v>142</v>
       </c>
-      <c r="C10" s="98" t="s">
+      <c r="C10" s="83" t="s">
         <v>143</v>
       </c>
-      <c r="D10" s="111" t="s">
+      <c r="D10" s="92" t="s">
         <v>144</v>
       </c>
-      <c r="E10" s="98">
+      <c r="E10" s="83">
         <v>3</v>
       </c>
-      <c r="F10" s="98">
+      <c r="F10" s="83">
         <v>3</v>
       </c>
-      <c r="G10" s="98">
+      <c r="G10" s="83">
         <v>3</v>
       </c>
-      <c r="H10" s="98">
+      <c r="H10" s="83">
         <v>3</v>
       </c>
-      <c r="I10" s="98">
+      <c r="I10" s="83">
         <v>3</v>
       </c>
-      <c r="J10" s="98">
+      <c r="J10" s="83">
         <v>3</v>
       </c>
-      <c r="K10" s="97" t="s">
+      <c r="K10" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="L10" s="97"/>
-      <c r="M10" s="97"/>
+      <c r="L10" s="82"/>
+      <c r="M10" s="82"/>
     </row>
     <row r="11" spans="1:13" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="63" t="s">
@@ -6666,299 +6675,299 @@
       <c r="L11" s="62"/>
       <c r="M11" s="62"/>
     </row>
-    <row r="12" spans="1:13" s="98" customFormat="1" ht="345" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="107" t="s">
+    <row r="12" spans="1:13" s="83" customFormat="1" ht="345" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="104" t="s">
         <v>146</v>
       </c>
-      <c r="C12" s="113" t="s">
+      <c r="C12" s="107" t="s">
         <v>147</v>
       </c>
-      <c r="D12" s="110" t="s">
+      <c r="D12" s="108" t="s">
         <v>148</v>
       </c>
-      <c r="E12" s="109">
+      <c r="E12" s="103">
         <v>15</v>
       </c>
-      <c r="F12" s="109">
+      <c r="F12" s="103">
         <v>15</v>
       </c>
-      <c r="G12" s="109">
+      <c r="G12" s="103">
         <v>15</v>
       </c>
-      <c r="H12" s="109">
+      <c r="H12" s="103">
         <v>10</v>
       </c>
-      <c r="I12" s="109">
+      <c r="I12" s="103">
         <v>10</v>
       </c>
-      <c r="J12" s="109">
+      <c r="J12" s="103">
         <v>10</v>
       </c>
-      <c r="K12" s="97" t="s">
+      <c r="K12" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="L12" s="97"/>
-      <c r="M12" s="97"/>
-    </row>
-    <row r="13" spans="1:13" s="98" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="107"/>
-      <c r="C13" s="113"/>
-      <c r="D13" s="110"/>
-      <c r="E13" s="109"/>
-      <c r="F13" s="109"/>
-      <c r="G13" s="109"/>
-      <c r="H13" s="109"/>
-      <c r="I13" s="109"/>
-      <c r="J13" s="109"/>
-      <c r="K13" s="97"/>
-      <c r="L13" s="97"/>
-      <c r="M13" s="97"/>
-    </row>
-    <row r="14" spans="1:13" s="98" customFormat="1" ht="255" x14ac:dyDescent="0.25">
-      <c r="B14" s="98" t="s">
+      <c r="L12" s="82"/>
+      <c r="M12" s="82"/>
+    </row>
+    <row r="13" spans="1:13" s="83" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="104"/>
+      <c r="C13" s="107"/>
+      <c r="D13" s="108"/>
+      <c r="E13" s="103"/>
+      <c r="F13" s="103"/>
+      <c r="G13" s="103"/>
+      <c r="H13" s="103"/>
+      <c r="I13" s="103"/>
+      <c r="J13" s="103"/>
+      <c r="K13" s="82"/>
+      <c r="L13" s="82"/>
+      <c r="M13" s="82"/>
+    </row>
+    <row r="14" spans="1:13" s="83" customFormat="1" ht="255" x14ac:dyDescent="0.25">
+      <c r="B14" s="83" t="s">
         <v>149</v>
       </c>
-      <c r="C14" s="98" t="s">
+      <c r="C14" s="83" t="s">
         <v>150</v>
       </c>
-      <c r="D14" s="111" t="s">
+      <c r="D14" s="92" t="s">
         <v>151</v>
       </c>
-      <c r="E14" s="98">
+      <c r="E14" s="83">
         <v>7</v>
       </c>
-      <c r="F14" s="98">
+      <c r="F14" s="83">
         <v>7</v>
       </c>
-      <c r="G14" s="98">
+      <c r="G14" s="83">
         <v>7</v>
       </c>
-      <c r="H14" s="98">
+      <c r="H14" s="83">
         <v>4</v>
       </c>
-      <c r="I14" s="98">
+      <c r="I14" s="83">
         <v>4</v>
       </c>
-      <c r="J14" s="98">
+      <c r="J14" s="83">
         <v>4</v>
       </c>
-      <c r="K14" s="97" t="s">
+      <c r="K14" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="L14" s="97"/>
-      <c r="M14" s="97"/>
-    </row>
-    <row r="15" spans="1:13" s="98" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="B15" s="98" t="s">
+      <c r="L14" s="82"/>
+      <c r="M14" s="82"/>
+    </row>
+    <row r="15" spans="1:13" s="83" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B15" s="83" t="s">
         <v>152</v>
       </c>
-      <c r="C15" s="98" t="s">
+      <c r="C15" s="83" t="s">
         <v>153</v>
       </c>
-      <c r="D15" s="112" t="s">
+      <c r="D15" s="93" t="s">
         <v>154</v>
       </c>
-      <c r="E15" s="98">
+      <c r="E15" s="83">
         <v>3</v>
       </c>
-      <c r="F15" s="98">
+      <c r="F15" s="83">
         <v>3</v>
       </c>
-      <c r="G15" s="98">
+      <c r="G15" s="83">
         <v>3</v>
       </c>
-      <c r="H15" s="98">
+      <c r="H15" s="83">
         <v>3</v>
       </c>
-      <c r="I15" s="98">
+      <c r="I15" s="83">
         <v>3</v>
       </c>
-      <c r="J15" s="98">
+      <c r="J15" s="83">
         <v>3</v>
       </c>
-      <c r="K15" s="97" t="s">
+      <c r="K15" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="L15" s="97"/>
-      <c r="M15" s="97"/>
-    </row>
-    <row r="16" spans="1:13" s="98" customFormat="1" ht="405" x14ac:dyDescent="0.25">
-      <c r="B16" s="98" t="s">
+      <c r="L15" s="82"/>
+      <c r="M15" s="82"/>
+    </row>
+    <row r="16" spans="1:13" s="83" customFormat="1" ht="405" x14ac:dyDescent="0.25">
+      <c r="B16" s="83" t="s">
         <v>155</v>
       </c>
-      <c r="C16" s="98" t="s">
+      <c r="C16" s="83" t="s">
         <v>156</v>
       </c>
-      <c r="D16" s="111" t="s">
+      <c r="D16" s="92" t="s">
         <v>157</v>
       </c>
-      <c r="E16" s="98">
+      <c r="E16" s="83">
         <v>7</v>
       </c>
-      <c r="F16" s="98">
+      <c r="F16" s="83">
         <v>7</v>
       </c>
-      <c r="G16" s="98">
+      <c r="G16" s="83">
         <v>7</v>
       </c>
-      <c r="H16" s="98">
+      <c r="H16" s="83">
         <v>4</v>
       </c>
-      <c r="I16" s="98">
+      <c r="I16" s="83">
         <v>4</v>
       </c>
-      <c r="J16" s="98">
+      <c r="J16" s="83">
         <v>4</v>
       </c>
-      <c r="K16" s="97" t="s">
+      <c r="K16" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="L16" s="97"/>
-      <c r="M16" s="97"/>
-    </row>
-    <row r="17" spans="1:13" s="98" customFormat="1" ht="270" x14ac:dyDescent="0.25">
-      <c r="B17" s="98" t="s">
+      <c r="L16" s="82"/>
+      <c r="M16" s="82"/>
+    </row>
+    <row r="17" spans="1:13" s="83" customFormat="1" ht="270" x14ac:dyDescent="0.25">
+      <c r="B17" s="83" t="s">
         <v>158</v>
       </c>
-      <c r="C17" s="98" t="s">
+      <c r="C17" s="83" t="s">
         <v>159</v>
       </c>
-      <c r="D17" s="111" t="s">
+      <c r="D17" s="92" t="s">
         <v>160</v>
       </c>
-      <c r="E17" s="98">
+      <c r="E17" s="83">
         <v>7</v>
       </c>
-      <c r="F17" s="98">
+      <c r="F17" s="83">
         <v>7</v>
       </c>
-      <c r="G17" s="98">
+      <c r="G17" s="83">
         <v>7</v>
       </c>
-      <c r="H17" s="98">
+      <c r="H17" s="83">
         <v>4</v>
       </c>
-      <c r="I17" s="98">
+      <c r="I17" s="83">
         <v>4</v>
       </c>
-      <c r="J17" s="98">
+      <c r="J17" s="83">
         <v>4</v>
       </c>
-      <c r="K17" s="97"/>
-      <c r="L17" s="97"/>
-      <c r="M17" s="97"/>
-    </row>
-    <row r="18" spans="1:13" s="98" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="109"/>
-      <c r="B18" s="107" t="s">
+      <c r="K17" s="82"/>
+      <c r="L17" s="82"/>
+      <c r="M17" s="82"/>
+    </row>
+    <row r="18" spans="1:13" s="83" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="103"/>
+      <c r="B18" s="104" t="s">
         <v>161</v>
       </c>
-      <c r="C18" s="107" t="s">
+      <c r="C18" s="104" t="s">
         <v>162</v>
       </c>
-      <c r="D18" s="114" t="s">
+      <c r="D18" s="101" t="s">
         <v>163</v>
       </c>
-      <c r="E18" s="109">
+      <c r="E18" s="103">
         <v>7</v>
       </c>
-      <c r="F18" s="109">
+      <c r="F18" s="103">
         <v>7</v>
       </c>
-      <c r="G18" s="109">
+      <c r="G18" s="103">
         <v>7</v>
       </c>
-      <c r="H18" s="109">
+      <c r="H18" s="103">
         <v>4</v>
       </c>
-      <c r="I18" s="109">
+      <c r="I18" s="103">
         <v>4</v>
       </c>
-      <c r="J18" s="109">
+      <c r="J18" s="103">
         <v>4</v>
       </c>
-      <c r="K18" s="97"/>
-      <c r="L18" s="97"/>
-      <c r="M18" s="97"/>
-    </row>
-    <row r="19" spans="1:13" s="98" customFormat="1" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="109"/>
-      <c r="B19" s="107"/>
-      <c r="C19" s="107"/>
-      <c r="D19" s="108"/>
-      <c r="E19" s="109"/>
-      <c r="F19" s="109"/>
-      <c r="G19" s="109"/>
-      <c r="H19" s="109"/>
-      <c r="I19" s="109"/>
-      <c r="J19" s="109"/>
-      <c r="K19" s="97"/>
-      <c r="L19" s="97"/>
-      <c r="M19" s="97"/>
-    </row>
-    <row r="20" spans="1:13" s="98" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="B20" s="98" t="s">
+      <c r="K18" s="82"/>
+      <c r="L18" s="82"/>
+      <c r="M18" s="82"/>
+    </row>
+    <row r="19" spans="1:13" s="83" customFormat="1" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="103"/>
+      <c r="B19" s="104"/>
+      <c r="C19" s="104"/>
+      <c r="D19" s="102"/>
+      <c r="E19" s="103"/>
+      <c r="F19" s="103"/>
+      <c r="G19" s="103"/>
+      <c r="H19" s="103"/>
+      <c r="I19" s="103"/>
+      <c r="J19" s="103"/>
+      <c r="K19" s="82"/>
+      <c r="L19" s="82"/>
+      <c r="M19" s="82"/>
+    </row>
+    <row r="20" spans="1:13" s="83" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="B20" s="83" t="s">
         <v>164</v>
       </c>
-      <c r="C20" s="98" t="s">
+      <c r="C20" s="83" t="s">
         <v>165</v>
       </c>
-      <c r="D20" s="111" t="s">
+      <c r="D20" s="92" t="s">
         <v>166</v>
       </c>
-      <c r="E20" s="98">
+      <c r="E20" s="83">
         <v>3</v>
       </c>
-      <c r="F20" s="98">
+      <c r="F20" s="83">
         <v>3</v>
       </c>
-      <c r="G20" s="98">
+      <c r="G20" s="83">
         <v>3</v>
       </c>
-      <c r="H20" s="98">
+      <c r="H20" s="83">
         <v>3</v>
       </c>
-      <c r="I20" s="98">
+      <c r="I20" s="83">
         <v>3</v>
       </c>
-      <c r="J20" s="98">
+      <c r="J20" s="83">
         <v>3</v>
       </c>
-      <c r="K20" s="97"/>
-      <c r="L20" s="97"/>
-      <c r="M20" s="97"/>
-    </row>
-    <row r="21" spans="1:13" s="98" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="B21" s="98" t="s">
+      <c r="K20" s="82"/>
+      <c r="L20" s="82"/>
+      <c r="M20" s="82"/>
+    </row>
+    <row r="21" spans="1:13" s="83" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="B21" s="83" t="s">
         <v>167</v>
       </c>
-      <c r="C21" s="98" t="s">
+      <c r="C21" s="83" t="s">
         <v>168</v>
       </c>
-      <c r="D21" s="112" t="s">
+      <c r="D21" s="93" t="s">
         <v>169</v>
       </c>
-      <c r="E21" s="98">
+      <c r="E21" s="83">
         <v>2</v>
       </c>
-      <c r="F21" s="98">
+      <c r="F21" s="83">
         <v>2</v>
       </c>
-      <c r="G21" s="98">
+      <c r="G21" s="83">
         <v>2</v>
       </c>
-      <c r="H21" s="98">
+      <c r="H21" s="83">
         <v>2</v>
       </c>
-      <c r="I21" s="98">
+      <c r="I21" s="83">
         <v>2</v>
       </c>
-      <c r="J21" s="98">
+      <c r="J21" s="83">
         <v>2</v>
       </c>
-      <c r="K21" s="97"/>
-      <c r="L21" s="97"/>
-      <c r="M21" s="97"/>
+      <c r="K21" s="82"/>
+      <c r="L21" s="82"/>
+      <c r="M21" s="82"/>
     </row>
     <row r="22" spans="1:13" s="11" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" s="44"/>
@@ -7001,165 +7010,165 @@
       <c r="L23" s="62"/>
       <c r="M23" s="62"/>
     </row>
-    <row r="24" spans="1:13" s="98" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="B24" s="98" t="s">
+    <row r="24" spans="1:13" s="83" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B24" s="83" t="s">
         <v>174</v>
       </c>
-      <c r="C24" s="98" t="s">
+      <c r="C24" s="83" t="s">
         <v>175</v>
       </c>
-      <c r="D24" s="112" t="s">
+      <c r="D24" s="93" t="s">
         <v>176</v>
       </c>
-      <c r="E24" s="98">
+      <c r="E24" s="83">
         <v>15</v>
       </c>
-      <c r="F24" s="98">
+      <c r="F24" s="83">
         <v>15</v>
       </c>
-      <c r="G24" s="98">
+      <c r="G24" s="83">
         <v>15</v>
       </c>
-      <c r="H24" s="98">
+      <c r="H24" s="83">
         <v>10</v>
       </c>
-      <c r="I24" s="98">
+      <c r="I24" s="83">
         <v>10</v>
       </c>
-      <c r="J24" s="98">
+      <c r="J24" s="83">
         <v>10</v>
       </c>
-      <c r="K24" s="97"/>
-      <c r="L24" s="97"/>
-      <c r="M24" s="97"/>
-    </row>
-    <row r="25" spans="1:13" s="98" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="B25" s="98" t="s">
+      <c r="K24" s="82"/>
+      <c r="L24" s="82"/>
+      <c r="M24" s="82"/>
+    </row>
+    <row r="25" spans="1:13" s="83" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="B25" s="83" t="s">
         <v>177</v>
       </c>
-      <c r="C25" s="98" t="s">
+      <c r="C25" s="83" t="s">
         <v>178</v>
       </c>
-      <c r="D25" s="111" t="s">
+      <c r="D25" s="92" t="s">
         <v>179</v>
       </c>
-      <c r="E25" s="98">
+      <c r="E25" s="83">
         <v>7</v>
       </c>
-      <c r="F25" s="98">
+      <c r="F25" s="83">
         <v>7</v>
       </c>
-      <c r="G25" s="98">
+      <c r="G25" s="83">
         <v>7</v>
       </c>
-      <c r="H25" s="98">
+      <c r="H25" s="83">
         <v>4</v>
       </c>
-      <c r="I25" s="98">
+      <c r="I25" s="83">
         <v>4</v>
       </c>
-      <c r="J25" s="98">
+      <c r="J25" s="83">
         <v>4</v>
       </c>
-      <c r="K25" s="97"/>
-      <c r="L25" s="97"/>
-      <c r="M25" s="97"/>
-    </row>
-    <row r="26" spans="1:13" s="98" customFormat="1" ht="388.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="98" t="s">
+      <c r="K25" s="82"/>
+      <c r="L25" s="82"/>
+      <c r="M25" s="82"/>
+    </row>
+    <row r="26" spans="1:13" s="83" customFormat="1" ht="388.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="83" t="s">
         <v>180</v>
       </c>
-      <c r="C26" s="98" t="s">
+      <c r="C26" s="83" t="s">
         <v>181</v>
       </c>
-      <c r="D26" s="112" t="s">
+      <c r="D26" s="93" t="s">
         <v>321</v>
       </c>
-      <c r="E26" s="98">
+      <c r="E26" s="83">
         <v>7</v>
       </c>
-      <c r="F26" s="98">
+      <c r="F26" s="83">
         <v>7</v>
       </c>
-      <c r="G26" s="98">
+      <c r="G26" s="83">
         <v>7</v>
       </c>
-      <c r="H26" s="98">
+      <c r="H26" s="83">
         <v>4</v>
       </c>
-      <c r="I26" s="98">
+      <c r="I26" s="83">
         <v>4</v>
       </c>
-      <c r="J26" s="98">
+      <c r="J26" s="83">
         <v>4</v>
       </c>
-      <c r="K26" s="97"/>
-      <c r="L26" s="97"/>
-      <c r="M26" s="97"/>
-    </row>
-    <row r="27" spans="1:13" s="98" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="B27" s="98" t="s">
+      <c r="K26" s="82"/>
+      <c r="L26" s="82"/>
+      <c r="M26" s="82"/>
+    </row>
+    <row r="27" spans="1:13" s="83" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B27" s="83" t="s">
         <v>182</v>
       </c>
-      <c r="C27" s="98" t="s">
+      <c r="C27" s="83" t="s">
         <v>183</v>
       </c>
-      <c r="D27" s="112" t="s">
+      <c r="D27" s="93" t="s">
         <v>184</v>
       </c>
-      <c r="E27" s="98">
+      <c r="E27" s="83">
         <v>3</v>
       </c>
-      <c r="F27" s="98">
+      <c r="F27" s="83">
         <v>3</v>
       </c>
-      <c r="G27" s="98">
+      <c r="G27" s="83">
         <v>3</v>
       </c>
-      <c r="H27" s="98">
+      <c r="H27" s="83">
         <v>3</v>
       </c>
-      <c r="I27" s="98">
+      <c r="I27" s="83">
         <v>3</v>
       </c>
-      <c r="J27" s="98">
+      <c r="J27" s="83">
         <v>3</v>
       </c>
-      <c r="K27" s="97"/>
-      <c r="L27" s="97"/>
-      <c r="M27" s="97"/>
-    </row>
-    <row r="28" spans="1:13" s="98" customFormat="1" ht="214.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="98" t="s">
+      <c r="K27" s="82"/>
+      <c r="L27" s="82"/>
+      <c r="M27" s="82"/>
+    </row>
+    <row r="28" spans="1:13" s="83" customFormat="1" ht="214.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="83" t="s">
         <v>185</v>
       </c>
-      <c r="C28" s="98" t="s">
+      <c r="C28" s="83" t="s">
         <v>186</v>
       </c>
-      <c r="D28" s="112" t="s">
+      <c r="D28" s="93" t="s">
         <v>322</v>
       </c>
-      <c r="E28" s="98">
+      <c r="E28" s="83">
         <v>7</v>
       </c>
-      <c r="F28" s="98">
+      <c r="F28" s="83">
         <v>7</v>
       </c>
-      <c r="G28" s="98">
+      <c r="G28" s="83">
         <v>7</v>
       </c>
-      <c r="H28" s="98">
+      <c r="H28" s="83">
         <v>5</v>
       </c>
-      <c r="I28" s="98">
+      <c r="I28" s="83">
         <v>5</v>
       </c>
-      <c r="J28" s="98">
+      <c r="J28" s="83">
         <v>5</v>
       </c>
-      <c r="K28" s="97"/>
-      <c r="L28" s="97"/>
-      <c r="M28" s="97"/>
+      <c r="K28" s="82"/>
+      <c r="L28" s="82"/>
+      <c r="M28" s="82"/>
     </row>
     <row r="29" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
@@ -7198,34 +7207,34 @@
       <c r="L30" s="62"/>
       <c r="M30" s="62"/>
     </row>
-    <row r="31" spans="1:13" s="98" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="98" t="s">
+    <row r="31" spans="1:13" s="83" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="83" t="s">
         <v>191</v>
       </c>
-      <c r="C31" s="98" t="s">
+      <c r="C31" s="83" t="s">
         <v>192</v>
       </c>
-      <c r="E31" s="98">
+      <c r="E31" s="83">
         <v>2</v>
       </c>
-      <c r="F31" s="98">
+      <c r="F31" s="83">
         <v>2</v>
       </c>
-      <c r="G31" s="98">
+      <c r="G31" s="83">
         <v>2</v>
       </c>
-      <c r="H31" s="98">
+      <c r="H31" s="83">
         <v>2</v>
       </c>
-      <c r="I31" s="98">
+      <c r="I31" s="83">
         <v>2</v>
       </c>
-      <c r="J31" s="98">
+      <c r="J31" s="83">
         <v>2</v>
       </c>
-      <c r="K31" s="97"/>
-      <c r="L31" s="97"/>
-      <c r="M31" s="97"/>
+      <c r="K31" s="82"/>
+      <c r="L31" s="82"/>
+      <c r="M31" s="82"/>
     </row>
     <row r="32" spans="1:13" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="63" t="s">
@@ -7235,98 +7244,98 @@
       <c r="L32" s="62"/>
       <c r="M32" s="62"/>
     </row>
-    <row r="33" spans="1:13" s="98" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B33" s="98" t="s">
+    <row r="33" spans="1:13" s="83" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B33" s="83" t="s">
         <v>194</v>
       </c>
-      <c r="C33" s="98" t="s">
+      <c r="C33" s="83" t="s">
         <v>195</v>
       </c>
-      <c r="E33" s="98">
+      <c r="E33" s="83">
         <v>4</v>
       </c>
-      <c r="F33" s="98">
+      <c r="F33" s="83">
         <v>4</v>
       </c>
-      <c r="G33" s="98">
+      <c r="G33" s="83">
         <v>4</v>
       </c>
-      <c r="H33" s="98">
+      <c r="H33" s="83">
         <v>4</v>
       </c>
-      <c r="I33" s="98">
+      <c r="I33" s="83">
         <v>4</v>
       </c>
-      <c r="J33" s="98">
+      <c r="J33" s="83">
         <v>4</v>
       </c>
-      <c r="K33" s="97"/>
-      <c r="L33" s="97"/>
-      <c r="M33" s="97"/>
-    </row>
-    <row r="34" spans="1:13" s="98" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="B34" s="98" t="s">
+      <c r="K33" s="82"/>
+      <c r="L33" s="82"/>
+      <c r="M33" s="82"/>
+    </row>
+    <row r="34" spans="1:13" s="83" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="B34" s="83" t="s">
         <v>196</v>
       </c>
-      <c r="C34" s="98" t="s">
+      <c r="C34" s="83" t="s">
         <v>197</v>
       </c>
-      <c r="D34" s="111" t="s">
+      <c r="D34" s="92" t="s">
         <v>198</v>
       </c>
-      <c r="E34" s="98">
+      <c r="E34" s="83">
         <v>10</v>
       </c>
-      <c r="F34" s="98">
+      <c r="F34" s="83">
         <v>10</v>
       </c>
-      <c r="G34" s="98">
+      <c r="G34" s="83">
         <v>10</v>
       </c>
-      <c r="H34" s="98">
+      <c r="H34" s="83">
         <v>7</v>
       </c>
-      <c r="I34" s="98">
+      <c r="I34" s="83">
         <v>7</v>
       </c>
-      <c r="J34" s="98">
+      <c r="J34" s="83">
         <v>7</v>
       </c>
-      <c r="K34" s="97"/>
-      <c r="L34" s="97"/>
-      <c r="M34" s="97"/>
-    </row>
-    <row r="35" spans="1:13" s="98" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="B35" s="98" t="s">
+      <c r="K34" s="82"/>
+      <c r="L34" s="82"/>
+      <c r="M34" s="82"/>
+    </row>
+    <row r="35" spans="1:13" s="83" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="B35" s="83" t="s">
         <v>199</v>
       </c>
-      <c r="C35" s="98" t="s">
+      <c r="C35" s="83" t="s">
         <v>200</v>
       </c>
-      <c r="D35" s="111" t="s">
+      <c r="D35" s="92" t="s">
         <v>201</v>
       </c>
-      <c r="E35" s="98">
+      <c r="E35" s="83">
         <v>5</v>
       </c>
-      <c r="F35" s="98">
+      <c r="F35" s="83">
         <v>5</v>
       </c>
-      <c r="G35" s="98">
+      <c r="G35" s="83">
         <v>5</v>
       </c>
-      <c r="H35" s="98">
+      <c r="H35" s="83">
         <v>3</v>
       </c>
-      <c r="I35" s="98">
+      <c r="I35" s="83">
         <v>3</v>
       </c>
-      <c r="J35" s="98">
+      <c r="J35" s="83">
         <v>3</v>
       </c>
-      <c r="K35" s="97"/>
-      <c r="L35" s="97"/>
-      <c r="M35" s="97"/>
+      <c r="K35" s="82"/>
+      <c r="L35" s="82"/>
+      <c r="M35" s="82"/>
     </row>
     <row r="36" spans="1:13" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="63" t="s">
@@ -7337,6 +7346,9 @@
       <c r="M36" s="62"/>
     </row>
     <row r="37" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>328</v>
+      </c>
       <c r="B37" s="2" t="s">
         <v>203</v>
       </c>
@@ -7398,6 +7410,9 @@
       <c r="M38" s="43"/>
     </row>
     <row r="39" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>329</v>
+      </c>
       <c r="B39" s="2" t="s">
         <v>209</v>
       </c>
@@ -8099,48 +8114,48 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:13" s="98" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="98" t="s">
+    <row r="63" spans="1:13" s="83" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="83" t="s">
         <v>273</v>
       </c>
-      <c r="C63" s="98" t="s">
+      <c r="C63" s="83" t="s">
         <v>274</v>
       </c>
-      <c r="E63" s="98">
-        <v>1</v>
-      </c>
-      <c r="F63" s="98">
-        <v>1</v>
-      </c>
-      <c r="G63" s="98">
-        <v>1</v>
-      </c>
-      <c r="H63" s="98">
-        <v>1</v>
-      </c>
-      <c r="I63" s="98">
-        <v>1</v>
-      </c>
-      <c r="J63" s="98">
-        <v>1</v>
-      </c>
-      <c r="K63" s="97"/>
-      <c r="L63" s="97"/>
-      <c r="M63" s="97"/>
+      <c r="E63" s="83">
+        <v>1</v>
+      </c>
+      <c r="F63" s="83">
+        <v>1</v>
+      </c>
+      <c r="G63" s="83">
+        <v>1</v>
+      </c>
+      <c r="H63" s="83">
+        <v>1</v>
+      </c>
+      <c r="I63" s="83">
+        <v>1</v>
+      </c>
+      <c r="J63" s="83">
+        <v>1</v>
+      </c>
+      <c r="K63" s="82"/>
+      <c r="L63" s="82"/>
+      <c r="M63" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="E1:F1"/>
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="L4:L5"/>
     <mergeCell ref="M4:M5"/>
@@ -8153,17 +8168,17 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="D4:D5"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3 M6:M51">
@@ -8189,9 +8204,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8211,18 +8226,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="84" t="s">
+      <c r="D1" s="96" t="s">
         <v>320</v>
       </c>
-      <c r="E1" s="85"/>
+      <c r="E1" s="97"/>
       <c r="F1" s="70">
         <f>SUM(F2:F999)</f>
         <v>31</v>
       </c>
-      <c r="G1" s="84" t="s">
+      <c r="G1" s="96" t="s">
         <v>323</v>
       </c>
-      <c r="H1" s="85"/>
+      <c r="H1" s="97"/>
       <c r="I1" s="70">
         <f>SUM(I2:I999)</f>
         <v>19</v>
@@ -8258,7 +8273,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="91" t="s">
         <v>278</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -8287,7 +8302,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="91" t="s">
         <v>281</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -8316,7 +8331,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="91" t="s">
         <v>284</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -8345,7 +8360,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="91" t="s">
         <v>287</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -8406,7 +8421,7 @@
       <c r="L7" s="43"/>
     </row>
     <row r="8" spans="1:12" ht="150" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="91" t="s">
         <v>293</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -8465,47 +8480,47 @@
       <c r="L9" s="43"/>
     </row>
     <row r="10" spans="1:12" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="93" t="s">
+      <c r="A10" s="113" t="s">
         <v>298</v>
       </c>
-      <c r="B10" s="90" t="s">
+      <c r="B10" s="112" t="s">
         <v>299</v>
       </c>
-      <c r="C10" s="90" t="s">
+      <c r="C10" s="112" t="s">
         <v>300</v>
       </c>
-      <c r="D10" s="95">
+      <c r="D10" s="111">
         <v>15</v>
       </c>
-      <c r="E10" s="95">
+      <c r="E10" s="111">
         <v>15</v>
       </c>
-      <c r="F10" s="95">
+      <c r="F10" s="111">
         <v>15</v>
       </c>
-      <c r="G10" s="96">
+      <c r="G10" s="115">
         <v>10</v>
       </c>
-      <c r="H10" s="94">
+      <c r="H10" s="114">
         <v>10</v>
       </c>
-      <c r="I10" s="94">
+      <c r="I10" s="114">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="93"/>
-      <c r="B11" s="90"/>
-      <c r="C11" s="90"/>
-      <c r="D11" s="95"/>
-      <c r="E11" s="95"/>
-      <c r="F11" s="95"/>
-      <c r="G11" s="96"/>
-      <c r="H11" s="94"/>
-      <c r="I11" s="94"/>
+      <c r="A11" s="113"/>
+      <c r="B11" s="112"/>
+      <c r="C11" s="112"/>
+      <c r="D11" s="111"/>
+      <c r="E11" s="111"/>
+      <c r="F11" s="111"/>
+      <c r="G11" s="115"/>
+      <c r="H11" s="114"/>
+      <c r="I11" s="114"/>
     </row>
     <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="91" t="s">
         <v>301</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -8592,14 +8607,14 @@
       <c r="L14" s="43"/>
     </row>
     <row r="25" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D25" s="95"/>
-      <c r="E25" s="95"/>
-      <c r="F25" s="95"/>
+      <c r="D25" s="111"/>
+      <c r="E25" s="111"/>
+      <c r="F25" s="111"/>
     </row>
     <row r="26" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D26" s="95"/>
-      <c r="E26" s="95"/>
-      <c r="F26" s="95"/>
+      <c r="D26" s="111"/>
+      <c r="E26" s="111"/>
+      <c r="F26" s="111"/>
     </row>
     <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" s="25"/>
@@ -8609,6 +8624,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
     <mergeCell ref="F25:F26"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="C10:C11"/>
@@ -8616,13 +8638,6 @@
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="E25:E26"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:H11"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J2:K50">

</xml_diff>

<commit_message>
Obtencion de Datos de Reporte de Inventario
</commit_message>
<xml_diff>
--- a/documentos/Propuesta y Actividades/Funcionalidad Actual A migrar Aldebaran.xlsx
+++ b/documentos/Propuesta y Actividades/Funcionalidad Actual A migrar Aldebaran.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="1710" windowWidth="29040" windowHeight="15840" tabRatio="881" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="3540" windowWidth="29040" windowHeight="15840" tabRatio="881" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tareas Generales" sheetId="27" r:id="rId1"/>
@@ -54,20 +54,10 @@
     <definedName name="TG_NuevoAlcance">'Tareas Generales'!$H$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -103,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="328">
   <si>
     <t>Descripción</t>
   </si>
@@ -1695,12 +1685,6 @@
   </si>
   <si>
     <t>Estimación Nuevo Alcance</t>
-  </si>
-  <si>
-    <t>javi</t>
-  </si>
-  <si>
-    <t>ADC</t>
   </si>
 </sst>
 </file>
@@ -2143,7 +2127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2400,6 +2384,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3841,20 +3828,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="94"/>
-      <c r="B1" s="95"/>
-      <c r="C1" s="96" t="s">
+      <c r="A1" s="95"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="97" t="s">
         <v>320</v>
       </c>
-      <c r="D1" s="97"/>
+      <c r="D1" s="98"/>
       <c r="E1" s="70">
         <f>SUM(E2:E7)</f>
         <v>57</v>
       </c>
-      <c r="F1" s="96" t="s">
+      <c r="F1" s="97" t="s">
         <v>327</v>
       </c>
-      <c r="G1" s="97"/>
+      <c r="G1" s="98"/>
       <c r="H1" s="70">
         <f>SUM(H2:H7)</f>
         <v>44</v>
@@ -4358,22 +4345,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="94"/>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="96" t="s">
+      <c r="A1" s="95"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="97" t="s">
         <v>320</v>
       </c>
-      <c r="F1" s="97"/>
+      <c r="F1" s="98"/>
       <c r="G1" s="70">
         <f>SUM(G3:G1000)</f>
         <v>53</v>
       </c>
-      <c r="H1" s="96" t="s">
+      <c r="H1" s="97" t="s">
         <v>323</v>
       </c>
-      <c r="I1" s="97"/>
+      <c r="I1" s="98"/>
       <c r="J1" s="70">
         <f>SUM(J3:J1000)</f>
         <v>23.000000000000004</v>
@@ -4435,7 +4422,7 @@
       <c r="C4" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="98" t="s">
+      <c r="D4" s="99" t="s">
         <v>22</v>
       </c>
       <c r="E4" s="84">
@@ -4467,7 +4454,7 @@
       <c r="C5" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="98"/>
+      <c r="D5" s="99"/>
       <c r="E5" s="84">
         <v>1</v>
       </c>
@@ -4497,7 +4484,7 @@
       <c r="C6" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="98"/>
+      <c r="D6" s="99"/>
       <c r="E6" s="84">
         <v>1</v>
       </c>
@@ -4700,7 +4687,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>317</v>
       </c>
@@ -4732,7 +4719,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="49" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="49" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" s="43"/>
       <c r="B14" s="44" t="s">
         <v>42</v>
@@ -4763,7 +4750,7 @@
       </c>
       <c r="K14" s="43"/>
     </row>
-    <row r="15" spans="1:11" s="82" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="82" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="B15" s="83" t="s">
         <v>44</v>
       </c>
@@ -4856,7 +4843,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="72"/>
       <c r="B18" s="73" t="s">
         <v>51</v>
@@ -4922,7 +4909,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="72"/>
       <c r="B20" s="73" t="s">
         <v>58</v>
@@ -5131,13 +5118,13 @@
       <c r="D27" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="E27" s="100">
+      <c r="E27" s="101">
         <v>4</v>
       </c>
-      <c r="F27" s="100">
+      <c r="F27" s="101">
         <v>3</v>
       </c>
-      <c r="G27" s="100">
+      <c r="G27" s="101">
         <v>3</v>
       </c>
       <c r="H27" s="19">
@@ -5162,9 +5149,9 @@
       <c r="D28" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="E28" s="100"/>
-      <c r="F28" s="100"/>
-      <c r="G28" s="100"/>
+      <c r="E28" s="101"/>
+      <c r="F28" s="101"/>
+      <c r="G28" s="101"/>
       <c r="H28" s="19">
         <v>0</v>
       </c>
@@ -5479,7 +5466,7 @@
       <c r="C41" s="83" t="s">
         <v>104</v>
       </c>
-      <c r="D41" s="98" t="s">
+      <c r="D41" s="99" t="s">
         <v>105</v>
       </c>
       <c r="E41" s="84">
@@ -5511,7 +5498,7 @@
       <c r="C42" s="83" t="s">
         <v>106</v>
       </c>
-      <c r="D42" s="98"/>
+      <c r="D42" s="99"/>
       <c r="E42" s="84">
         <v>1</v>
       </c>
@@ -5541,7 +5528,7 @@
       <c r="C43" s="83" t="s">
         <v>108</v>
       </c>
-      <c r="D43" s="98"/>
+      <c r="D43" s="99"/>
       <c r="E43" s="84">
         <v>1</v>
       </c>
@@ -6366,7 +6353,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
+      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6388,22 +6375,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="105"/>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="109" t="s">
+      <c r="A1" s="106"/>
+      <c r="B1" s="106"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="110" t="s">
         <v>320</v>
       </c>
-      <c r="F1" s="110"/>
+      <c r="F1" s="111"/>
       <c r="G1" s="71">
         <f>SUM(G2:G1000)</f>
         <v>207</v>
       </c>
-      <c r="H1" s="109" t="s">
+      <c r="H1" s="110" t="s">
         <v>323</v>
       </c>
-      <c r="I1" s="110"/>
+      <c r="I1" s="111"/>
       <c r="J1" s="71">
         <f>SUM(J2:J1000)</f>
         <v>131</v>
@@ -6450,52 +6437,52 @@
       <c r="M3" s="62"/>
     </row>
     <row r="4" spans="1:13" s="83" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="104" t="s">
+      <c r="B4" s="105" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="104" t="s">
+      <c r="C4" s="105" t="s">
         <v>128</v>
       </c>
-      <c r="D4" s="102" t="s">
+      <c r="D4" s="103" t="s">
         <v>129</v>
       </c>
-      <c r="E4" s="103">
+      <c r="E4" s="104">
         <v>10</v>
       </c>
-      <c r="F4" s="103">
+      <c r="F4" s="104">
         <v>15</v>
       </c>
-      <c r="G4" s="103">
+      <c r="G4" s="104">
         <v>15</v>
       </c>
-      <c r="H4" s="103">
+      <c r="H4" s="104">
         <v>10</v>
       </c>
-      <c r="I4" s="103">
+      <c r="I4" s="104">
         <v>10</v>
       </c>
-      <c r="J4" s="103">
+      <c r="J4" s="104">
         <v>10</v>
       </c>
-      <c r="K4" s="103" t="s">
+      <c r="K4" s="104" t="s">
         <v>57</v>
       </c>
-      <c r="L4" s="103"/>
-      <c r="M4" s="103"/>
+      <c r="L4" s="104"/>
+      <c r="M4" s="104"/>
     </row>
     <row r="5" spans="1:13" s="83" customFormat="1" ht="272.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="104"/>
-      <c r="C5" s="104"/>
-      <c r="D5" s="108"/>
-      <c r="E5" s="103"/>
-      <c r="F5" s="103"/>
-      <c r="G5" s="103"/>
-      <c r="H5" s="103"/>
-      <c r="I5" s="103"/>
-      <c r="J5" s="103"/>
-      <c r="K5" s="103"/>
-      <c r="L5" s="103"/>
-      <c r="M5" s="103"/>
+      <c r="B5" s="105"/>
+      <c r="C5" s="105"/>
+      <c r="D5" s="109"/>
+      <c r="E5" s="104"/>
+      <c r="F5" s="104"/>
+      <c r="G5" s="104"/>
+      <c r="H5" s="104"/>
+      <c r="I5" s="104"/>
+      <c r="J5" s="104"/>
+      <c r="K5" s="104"/>
+      <c r="L5" s="104"/>
+      <c r="M5" s="104"/>
     </row>
     <row r="6" spans="1:13" s="83" customFormat="1" ht="300" x14ac:dyDescent="0.25">
       <c r="B6" s="83" t="s">
@@ -6676,31 +6663,31 @@
       <c r="M11" s="62"/>
     </row>
     <row r="12" spans="1:13" s="83" customFormat="1" ht="345" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="104" t="s">
+      <c r="B12" s="105" t="s">
         <v>146</v>
       </c>
-      <c r="C12" s="107" t="s">
+      <c r="C12" s="108" t="s">
         <v>147</v>
       </c>
-      <c r="D12" s="108" t="s">
+      <c r="D12" s="109" t="s">
         <v>148</v>
       </c>
-      <c r="E12" s="103">
+      <c r="E12" s="104">
         <v>15</v>
       </c>
-      <c r="F12" s="103">
+      <c r="F12" s="104">
         <v>15</v>
       </c>
-      <c r="G12" s="103">
+      <c r="G12" s="104">
         <v>15</v>
       </c>
-      <c r="H12" s="103">
+      <c r="H12" s="104">
         <v>10</v>
       </c>
-      <c r="I12" s="103">
+      <c r="I12" s="104">
         <v>10</v>
       </c>
-      <c r="J12" s="103">
+      <c r="J12" s="104">
         <v>10</v>
       </c>
       <c r="K12" s="82" t="s">
@@ -6710,15 +6697,15 @@
       <c r="M12" s="82"/>
     </row>
     <row r="13" spans="1:13" s="83" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="104"/>
-      <c r="C13" s="107"/>
-      <c r="D13" s="108"/>
-      <c r="E13" s="103"/>
-      <c r="F13" s="103"/>
-      <c r="G13" s="103"/>
-      <c r="H13" s="103"/>
-      <c r="I13" s="103"/>
-      <c r="J13" s="103"/>
+      <c r="B13" s="105"/>
+      <c r="C13" s="108"/>
+      <c r="D13" s="109"/>
+      <c r="E13" s="104"/>
+      <c r="F13" s="104"/>
+      <c r="G13" s="104"/>
+      <c r="H13" s="104"/>
+      <c r="I13" s="104"/>
+      <c r="J13" s="104"/>
       <c r="K13" s="82"/>
       <c r="L13" s="82"/>
       <c r="M13" s="82"/>
@@ -6858,32 +6845,32 @@
       <c r="M17" s="82"/>
     </row>
     <row r="18" spans="1:13" s="83" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="103"/>
-      <c r="B18" s="104" t="s">
+      <c r="A18" s="104"/>
+      <c r="B18" s="105" t="s">
         <v>161</v>
       </c>
-      <c r="C18" s="104" t="s">
+      <c r="C18" s="105" t="s">
         <v>162</v>
       </c>
-      <c r="D18" s="101" t="s">
+      <c r="D18" s="102" t="s">
         <v>163</v>
       </c>
-      <c r="E18" s="103">
+      <c r="E18" s="104">
         <v>7</v>
       </c>
-      <c r="F18" s="103">
+      <c r="F18" s="104">
         <v>7</v>
       </c>
-      <c r="G18" s="103">
+      <c r="G18" s="104">
         <v>7</v>
       </c>
-      <c r="H18" s="103">
+      <c r="H18" s="104">
         <v>4</v>
       </c>
-      <c r="I18" s="103">
+      <c r="I18" s="104">
         <v>4</v>
       </c>
-      <c r="J18" s="103">
+      <c r="J18" s="104">
         <v>4</v>
       </c>
       <c r="K18" s="82"/>
@@ -6891,16 +6878,16 @@
       <c r="M18" s="82"/>
     </row>
     <row r="19" spans="1:13" s="83" customFormat="1" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="103"/>
-      <c r="B19" s="104"/>
-      <c r="C19" s="104"/>
-      <c r="D19" s="102"/>
-      <c r="E19" s="103"/>
-      <c r="F19" s="103"/>
-      <c r="G19" s="103"/>
-      <c r="H19" s="103"/>
-      <c r="I19" s="103"/>
-      <c r="J19" s="103"/>
+      <c r="A19" s="104"/>
+      <c r="B19" s="105"/>
+      <c r="C19" s="105"/>
+      <c r="D19" s="103"/>
+      <c r="E19" s="104"/>
+      <c r="F19" s="104"/>
+      <c r="G19" s="104"/>
+      <c r="H19" s="104"/>
+      <c r="I19" s="104"/>
+      <c r="J19" s="104"/>
       <c r="K19" s="82"/>
       <c r="L19" s="82"/>
       <c r="M19" s="82"/>
@@ -7346,10 +7333,7 @@
       <c r="M36" s="62"/>
     </row>
     <row r="37" spans="1:13" ht="120" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="94" t="s">
         <v>203</v>
       </c>
       <c r="C37" s="2" t="s">
@@ -7410,10 +7394,7 @@
       <c r="M38" s="43"/>
     </row>
     <row r="39" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="94" t="s">
         <v>209</v>
       </c>
       <c r="C39" s="2" t="s">
@@ -7442,7 +7423,7 @@
       </c>
     </row>
     <row r="40" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="94" t="s">
         <v>212</v>
       </c>
       <c r="C40" s="2" t="s">
@@ -7535,7 +7516,7 @@
       <c r="M42" s="43"/>
     </row>
     <row r="43" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="94" t="s">
         <v>221</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -8226,18 +8207,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="96" t="s">
+      <c r="D1" s="97" t="s">
         <v>320</v>
       </c>
-      <c r="E1" s="97"/>
+      <c r="E1" s="98"/>
       <c r="F1" s="70">
         <f>SUM(F2:F999)</f>
         <v>31</v>
       </c>
-      <c r="G1" s="96" t="s">
+      <c r="G1" s="97" t="s">
         <v>323</v>
       </c>
-      <c r="H1" s="97"/>
+      <c r="H1" s="98"/>
       <c r="I1" s="70">
         <f>SUM(I2:I999)</f>
         <v>19</v>
@@ -8480,44 +8461,44 @@
       <c r="L9" s="43"/>
     </row>
     <row r="10" spans="1:12" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="113" t="s">
+      <c r="A10" s="114" t="s">
         <v>298</v>
       </c>
-      <c r="B10" s="112" t="s">
+      <c r="B10" s="113" t="s">
         <v>299</v>
       </c>
-      <c r="C10" s="112" t="s">
+      <c r="C10" s="113" t="s">
         <v>300</v>
       </c>
-      <c r="D10" s="111">
+      <c r="D10" s="112">
         <v>15</v>
       </c>
-      <c r="E10" s="111">
+      <c r="E10" s="112">
         <v>15</v>
       </c>
-      <c r="F10" s="111">
+      <c r="F10" s="112">
         <v>15</v>
       </c>
-      <c r="G10" s="115">
+      <c r="G10" s="116">
         <v>10</v>
       </c>
-      <c r="H10" s="114">
+      <c r="H10" s="115">
         <v>10</v>
       </c>
-      <c r="I10" s="114">
+      <c r="I10" s="115">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="113"/>
-      <c r="B11" s="112"/>
-      <c r="C11" s="112"/>
-      <c r="D11" s="111"/>
-      <c r="E11" s="111"/>
-      <c r="F11" s="111"/>
-      <c r="G11" s="115"/>
-      <c r="H11" s="114"/>
-      <c r="I11" s="114"/>
+      <c r="A11" s="114"/>
+      <c r="B11" s="113"/>
+      <c r="C11" s="113"/>
+      <c r="D11" s="112"/>
+      <c r="E11" s="112"/>
+      <c r="F11" s="112"/>
+      <c r="G11" s="116"/>
+      <c r="H11" s="115"/>
+      <c r="I11" s="115"/>
     </row>
     <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="91" t="s">
@@ -8607,14 +8588,14 @@
       <c r="L14" s="43"/>
     </row>
     <row r="25" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D25" s="111"/>
-      <c r="E25" s="111"/>
-      <c r="F25" s="111"/>
+      <c r="D25" s="112"/>
+      <c r="E25" s="112"/>
+      <c r="F25" s="112"/>
     </row>
     <row r="26" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D26" s="111"/>
-      <c r="E26" s="111"/>
-      <c r="F26" s="111"/>
+      <c r="D26" s="112"/>
+      <c r="E26" s="112"/>
+      <c r="F26" s="112"/>
     </row>
     <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" s="25"/>

</xml_diff>